<commit_message>
move all tool to same dir
</commit_message>
<xml_diff>
--- a/Configs/excels/Demo.xlsx
+++ b/Configs/excels/Demo.xlsx
@@ -1,28 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="NPC" sheetId="1" r:id="rId1"/>
+    <sheet name="@Types" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skills</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>repeated int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RepeatCheck:true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MakeIndex:true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ListSpliter:","</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npc1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血量上限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TableName: "NPC" Package: "table" CSClassHeader: "[System.Serializable]"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -50,15 +134,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,37 +432,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="24.75" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>10001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>